<commit_message>
Aggiornamenti lint + eccezioni
</commit_message>
<xml_diff>
--- a/Results/Results.xlsx
+++ b/Results/Results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/federicaventriglia/Documents/Universita/TESI/EspressoTests/EspressoTests/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A6E0551-8058-CF4A-A3F9-854F1C9C7338}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE2E784F-81C9-E546-9643-5B89AAF9B960}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25640" windowHeight="19480" xr2:uid="{262774B7-AB6E-2E48-BB18-D4F78B06E237}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27740" windowHeight="19480" xr2:uid="{262774B7-AB6E-2E48-BB18-D4F78B06E237}"/>
   </bookViews>
   <sheets>
     <sheet name="Total" sheetId="7" r:id="rId1"/>
@@ -13376,8 +13376,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A92B7623-75A6-7B46-8147-ADF8D32CC273}">
   <dimension ref="A1:AQ20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="73" workbookViewId="0">
-      <selection activeCell="AO9" sqref="AO9"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="73" workbookViewId="0">
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -14306,6 +14306,40 @@
       <c r="AO8" s="13">
         <f>AVERAGE(AO2:AO7)</f>
         <v>0.51666666666666672</v>
+      </c>
+    </row>
+    <row r="9" spans="1:43">
+      <c r="H9">
+        <f>SUM(H2:H7)</f>
+        <v>51</v>
+      </c>
+      <c r="M9">
+        <f t="shared" ref="I9:AO9" si="3">SUM(M2:M7)</f>
+        <v>29</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="3"/>
+        <v>52</v>
+      </c>
+      <c r="W9">
+        <f t="shared" si="3"/>
+        <v>33</v>
+      </c>
+      <c r="Z9">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AC9">
+        <f t="shared" si="3"/>
+        <v>35</v>
+      </c>
+      <c r="AH9">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="AM9">
+        <f t="shared" si="3"/>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:43" ht="20">

</xml_diff>